<commit_message>
ISSUE #7: Made 24 phrases for rainy weather in the 32-49 degree range.
Also edited the Xcode storyboard a bit. The constraints are currently broken. They don't need to be fixed yet.
</commit_message>
<xml_diff>
--- a/Planning Files/punchy_phrases.xlsx
+++ b/Planning Files/punchy_phrases.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="48">
   <si>
     <t>Category</t>
   </si>
@@ -77,16 +77,100 @@
     <t>-</t>
   </si>
   <si>
-    <t>Note: character limit of</t>
-  </si>
-  <si>
     <t>Target athletes?</t>
   </si>
   <si>
     <t>Siri integration? What should I wear.</t>
   </si>
   <si>
-    <t>0 - 32º</t>
+    <t xml:space="preserve">32 - 49 </t>
+  </si>
+  <si>
+    <t>Note: character limit of about 45.</t>
+  </si>
+  <si>
+    <t>It's very cold and rainy. Heavy raincoat.</t>
+  </si>
+  <si>
+    <t>It's colder than the polar bear's toenails.</t>
+  </si>
+  <si>
+    <t>Extras</t>
+  </si>
+  <si>
+    <t>Colder than a penguin's ass. Dress heavy.</t>
+  </si>
+  <si>
+    <t>It's cold as hell and wet. Wear a coat.</t>
+  </si>
+  <si>
+    <t>Wear something water-resistant and warm.</t>
+  </si>
+  <si>
+    <t>I'd wear the opposite of a tank top.</t>
+  </si>
+  <si>
+    <t>Wear a coat, pack an umbrella. You'll need it.</t>
+  </si>
+  <si>
+    <t>Super rainy. Just stay inside.</t>
+  </si>
+  <si>
+    <t>Cold and rainy. Great day for some Netflix.</t>
+  </si>
+  <si>
+    <t>Work days vs. Saturday/Sunday detections.</t>
+  </si>
+  <si>
+    <t>Don't go out unless you love being drenched.</t>
+  </si>
+  <si>
+    <t>Umbrella would probably break. Big indoors day.</t>
+  </si>
+  <si>
+    <t>Not even rain boots would help at this point.</t>
+  </si>
+  <si>
+    <t>Are you a polar bear? Then stay inside.</t>
+  </si>
+  <si>
+    <t>Netflix is calling your name. Stay dry.</t>
+  </si>
+  <si>
+    <t>A little rainy. Dress warm, boots ideal.</t>
+  </si>
+  <si>
+    <t>You won't get too wet. It's cold though.</t>
+  </si>
+  <si>
+    <t>Pretty nippy. Layer up.</t>
+  </si>
+  <si>
+    <t>Not the worst, but it's kinda rainy.</t>
+  </si>
+  <si>
+    <t>Raincoat or a Patagonia should do.</t>
+  </si>
+  <si>
+    <t>Chilly and a bit wet. You know what to do.</t>
+  </si>
+  <si>
+    <t>Stay inside if you're sane.</t>
+  </si>
+  <si>
+    <t>Get your dog inside and don't leave for a bit.</t>
+  </si>
+  <si>
+    <t>Currently raining very heavily. Raincoat.</t>
+  </si>
+  <si>
+    <t>Unless you like bad weather, chill indoors.</t>
+  </si>
+  <si>
+    <t>Torrential downpour. No need to leave the house.</t>
+  </si>
+  <si>
+    <t>These can be grouped together, probably.</t>
   </si>
 </sst>
 </file>
@@ -155,7 +239,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -171,6 +255,11 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -453,21 +542,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M36"/>
+  <dimension ref="A1:O36"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20" style="1" customWidth="1"/>
     <col min="2" max="2" width="18.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.83203125" style="1" customWidth="1"/>
+    <col min="3" max="5" width="51.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.83203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="16.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="41.1640625" style="1" customWidth="1"/>
     <col min="8" max="8" width="16.33203125" style="1" customWidth="1"/>
     <col min="9" max="9" width="15" style="1" customWidth="1"/>
     <col min="10" max="10" width="13.1640625" style="1" customWidth="1"/>
@@ -477,17 +564,20 @@
     <col min="14" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="D2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="J2" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -498,10 +588,10 @@
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -513,7 +603,7 @@
       <c r="I4" s="2"/>
       <c r="J4" s="7"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>12</v>
       </c>
@@ -529,7 +619,7 @@
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -540,7 +630,7 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -551,7 +641,7 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
@@ -591,8 +681,11 @@
       <c r="M8" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O8" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
@@ -633,7 +726,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
@@ -650,80 +743,155 @@
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" s="10"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" s="10"/>
+      <c r="J12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="O12" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="2"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="2"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A16" s="2"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
+        <v>18</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="G13" s="10"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G14" s="10"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G15" s="10"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="G16" s="10"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
-      <c r="B17" s="3"/>
+      <c r="B17" s="8"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
-      <c r="B18" s="3"/>
+      <c r="B18" s="8"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
-      <c r="B19" s="3"/>
+      <c r="B19" s="8"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
-      <c r="B20" s="3"/>
+      <c r="B20" s="8"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
+      <c r="B21" s="9"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
+      <c r="B22" s="9"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
+      <c r="B23" s="9"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
@@ -765,6 +933,14 @@
       <c r="A36" s="2"/>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ISSUE #6: Fixed 'Ask for location' bug.
To an extent. It now only loads the UI after location access is granted. Need to brush it up, though.
</commit_message>
<xml_diff>
--- a/Planning Files/punchy_phrases.xlsx
+++ b/Planning Files/punchy_phrases.xlsx
@@ -742,8 +742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA36"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="D1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" showRuler="0" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
ISSUE #14: Started creating data model for phrases at bottom of screen.
</commit_message>
<xml_diff>
--- a/Planning Files/punchy_phrases.xlsx
+++ b/Planning Files/punchy_phrases.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="14400" windowHeight="17060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -369,6 +369,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="\&quot;@\&quot;\,"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -431,7 +434,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -456,9 +459,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -742,15 +751,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA36"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="H1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11:M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20" style="1" customWidth="1"/>
     <col min="2" max="2" width="18.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="54.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="65.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="54" style="1" customWidth="1"/>
     <col min="5" max="5" width="51.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.83203125" style="1" customWidth="1"/>
@@ -1055,37 +1064,37 @@
         <v>18</v>
       </c>
       <c r="B11" s="8"/>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="F11" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="G11" s="12"/>
-      <c r="H11" s="10" t="s">
+      <c r="G11" s="13"/>
+      <c r="H11" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="I11" s="12" t="s">
+      <c r="I11" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12" t="s">
+      <c r="J11" s="13"/>
+      <c r="K11" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="L11" s="12"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="8"/>
-      <c r="O11" s="8"/>
-      <c r="P11" s="8"/>
-      <c r="Q11" s="8"/>
-      <c r="R11" s="8"/>
-      <c r="S11" s="8"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="15"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="15"/>
+      <c r="R11" s="15"/>
+      <c r="S11" s="15"/>
       <c r="T11" s="8"/>
       <c r="U11" s="8"/>
       <c r="V11" s="8"/>
@@ -1100,39 +1109,39 @@
         <v>18</v>
       </c>
       <c r="B12" s="8"/>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="F12" s="12" t="s">
+      <c r="F12" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="G12" s="12"/>
-      <c r="H12" s="10" t="s">
+      <c r="G12" s="13"/>
+      <c r="H12" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="I12" s="12" t="s">
+      <c r="I12" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12" t="s">
+      <c r="J12" s="13"/>
+      <c r="K12" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="L12" s="12"/>
-      <c r="M12" s="12"/>
-      <c r="N12" s="8"/>
-      <c r="O12" s="7" t="s">
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="P12" s="8"/>
-      <c r="Q12" s="8"/>
-      <c r="R12" s="8"/>
-      <c r="S12" s="8"/>
+      <c r="P12" s="15"/>
+      <c r="Q12" s="15"/>
+      <c r="R12" s="15"/>
+      <c r="S12" s="15"/>
       <c r="T12" s="8"/>
       <c r="U12" s="8"/>
       <c r="V12" s="8"/>
@@ -1147,37 +1156,37 @@
         <v>18</v>
       </c>
       <c r="B13" s="8"/>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="F13" s="12" t="s">
+      <c r="F13" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="G13" s="12"/>
-      <c r="H13" s="10" t="s">
+      <c r="G13" s="13"/>
+      <c r="H13" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="I13" s="12" t="s">
+      <c r="I13" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12" t="s">
+      <c r="J13" s="13"/>
+      <c r="K13" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="L13" s="12"/>
-      <c r="M13" s="12"/>
-      <c r="N13" s="8"/>
-      <c r="O13" s="8"/>
-      <c r="P13" s="8"/>
-      <c r="Q13" s="8"/>
-      <c r="R13" s="8"/>
-      <c r="S13" s="8"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="15"/>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="15"/>
+      <c r="R13" s="15"/>
+      <c r="S13" s="15"/>
       <c r="T13" s="8"/>
       <c r="U13" s="8"/>
       <c r="V13" s="8"/>
@@ -1192,37 +1201,37 @@
         <v>18</v>
       </c>
       <c r="B14" s="8"/>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E14" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="F14" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="G14" s="12"/>
-      <c r="H14" s="10" t="s">
+      <c r="G14" s="13"/>
+      <c r="H14" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="I14" s="12" t="s">
+      <c r="I14" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12" t="s">
+      <c r="J14" s="13"/>
+      <c r="K14" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="L14" s="12"/>
-      <c r="M14" s="12"/>
-      <c r="N14" s="8"/>
-      <c r="O14" s="8"/>
-      <c r="P14" s="8"/>
-      <c r="Q14" s="8"/>
-      <c r="R14" s="8"/>
-      <c r="S14" s="8"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="15"/>
+      <c r="O14" s="15"/>
+      <c r="P14" s="15"/>
+      <c r="Q14" s="15"/>
+      <c r="R14" s="15"/>
+      <c r="S14" s="15"/>
       <c r="T14" s="8"/>
       <c r="U14" s="8"/>
       <c r="V14" s="8"/>
@@ -1237,37 +1246,37 @@
         <v>18</v>
       </c>
       <c r="B15" s="8"/>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E15" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F15" s="12" t="s">
+      <c r="F15" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="G15" s="12"/>
-      <c r="H15" s="10" t="s">
+      <c r="G15" s="13"/>
+      <c r="H15" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="I15" s="12" t="s">
+      <c r="I15" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12" t="s">
+      <c r="J15" s="13"/>
+      <c r="K15" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="L15" s="12"/>
-      <c r="M15" s="12"/>
-      <c r="N15" s="8"/>
-      <c r="O15" s="8"/>
-      <c r="P15" s="8"/>
-      <c r="Q15" s="8"/>
-      <c r="R15" s="8"/>
-      <c r="S15" s="8"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="15"/>
+      <c r="O15" s="15"/>
+      <c r="P15" s="15"/>
+      <c r="Q15" s="15"/>
+      <c r="R15" s="15"/>
+      <c r="S15" s="15"/>
       <c r="T15" s="8"/>
       <c r="U15" s="8"/>
       <c r="V15" s="8"/>
@@ -1282,37 +1291,37 @@
         <v>18</v>
       </c>
       <c r="B16" s="8"/>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="E16" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="F16" s="12" t="s">
+      <c r="F16" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="G16" s="12"/>
-      <c r="H16" s="10" t="s">
+      <c r="G16" s="13"/>
+      <c r="H16" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="I16" s="12" t="s">
+      <c r="I16" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12" t="s">
+      <c r="J16" s="13"/>
+      <c r="K16" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="L16" s="12"/>
-      <c r="M16" s="12"/>
-      <c r="N16" s="8"/>
-      <c r="O16" s="8"/>
-      <c r="P16" s="8"/>
-      <c r="Q16" s="8"/>
-      <c r="R16" s="8"/>
-      <c r="S16" s="8"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="13"/>
+      <c r="N16" s="15"/>
+      <c r="O16" s="15"/>
+      <c r="P16" s="15"/>
+      <c r="Q16" s="15"/>
+      <c r="R16" s="15"/>
+      <c r="S16" s="15"/>
       <c r="T16" s="8"/>
       <c r="U16" s="8"/>
       <c r="V16" s="8"/>
@@ -1327,37 +1336,37 @@
         <v>111</v>
       </c>
       <c r="B17" s="7"/>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="E17" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="F17" s="8" t="s">
+      <c r="F17" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="G17" s="8"/>
-      <c r="H17" s="10" t="s">
+      <c r="G17" s="15"/>
+      <c r="H17" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="I17" s="8" t="s">
+      <c r="I17" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="J17" s="8"/>
-      <c r="K17" s="12" t="s">
+      <c r="J17" s="15"/>
+      <c r="K17" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="L17" s="12"/>
-      <c r="M17" s="12"/>
-      <c r="N17" s="8"/>
-      <c r="O17" s="8"/>
-      <c r="P17" s="8"/>
-      <c r="Q17" s="8"/>
-      <c r="R17" s="8"/>
-      <c r="S17" s="8"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="13"/>
+      <c r="N17" s="15"/>
+      <c r="O17" s="15"/>
+      <c r="P17" s="15"/>
+      <c r="Q17" s="15"/>
+      <c r="R17" s="15"/>
+      <c r="S17" s="15"/>
       <c r="T17" s="8"/>
       <c r="U17" s="8"/>
       <c r="V17" s="8"/>
@@ -1372,37 +1381,37 @@
         <v>111</v>
       </c>
       <c r="B18" s="7"/>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="E18" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="F18" s="8" t="s">
+      <c r="F18" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="G18" s="8"/>
-      <c r="H18" s="10" t="s">
+      <c r="G18" s="15"/>
+      <c r="H18" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="I18" s="8" t="s">
+      <c r="I18" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="J18" s="8"/>
-      <c r="K18" s="12" t="s">
+      <c r="J18" s="15"/>
+      <c r="K18" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="L18" s="12"/>
-      <c r="M18" s="12"/>
-      <c r="N18" s="8"/>
-      <c r="O18" s="8"/>
-      <c r="P18" s="8"/>
-      <c r="Q18" s="8"/>
-      <c r="R18" s="8"/>
-      <c r="S18" s="8"/>
+      <c r="L18" s="13"/>
+      <c r="M18" s="13"/>
+      <c r="N18" s="15"/>
+      <c r="O18" s="15"/>
+      <c r="P18" s="15"/>
+      <c r="Q18" s="15"/>
+      <c r="R18" s="15"/>
+      <c r="S18" s="15"/>
       <c r="T18" s="8"/>
       <c r="U18" s="8"/>
       <c r="V18" s="8"/>
@@ -1417,37 +1426,37 @@
         <v>111</v>
       </c>
       <c r="B19" s="7"/>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="E19" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="F19" s="8" t="s">
+      <c r="F19" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="G19" s="8"/>
-      <c r="H19" s="10" t="s">
+      <c r="G19" s="15"/>
+      <c r="H19" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="I19" s="8" t="s">
+      <c r="I19" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="J19" s="8"/>
-      <c r="K19" s="12" t="s">
+      <c r="J19" s="15"/>
+      <c r="K19" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="L19" s="12"/>
-      <c r="M19" s="12"/>
-      <c r="N19" s="8"/>
-      <c r="O19" s="8"/>
-      <c r="P19" s="8"/>
-      <c r="Q19" s="8"/>
-      <c r="R19" s="8"/>
-      <c r="S19" s="8"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="13"/>
+      <c r="N19" s="15"/>
+      <c r="O19" s="15"/>
+      <c r="P19" s="15"/>
+      <c r="Q19" s="15"/>
+      <c r="R19" s="15"/>
+      <c r="S19" s="15"/>
       <c r="T19" s="8"/>
       <c r="U19" s="8"/>
       <c r="V19" s="8"/>
@@ -1462,37 +1471,37 @@
         <v>111</v>
       </c>
       <c r="B20" s="7"/>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E20" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="F20" s="8" t="s">
+      <c r="F20" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="G20" s="8"/>
-      <c r="H20" s="10" t="s">
+      <c r="G20" s="15"/>
+      <c r="H20" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="I20" s="8" t="s">
+      <c r="I20" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="J20" s="8"/>
-      <c r="K20" s="12" t="s">
+      <c r="J20" s="15"/>
+      <c r="K20" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="L20" s="12"/>
-      <c r="M20" s="12"/>
-      <c r="N20" s="8"/>
-      <c r="O20" s="8"/>
-      <c r="P20" s="8"/>
-      <c r="Q20" s="8"/>
-      <c r="R20" s="8"/>
-      <c r="S20" s="8"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="13"/>
+      <c r="N20" s="15"/>
+      <c r="O20" s="15"/>
+      <c r="P20" s="15"/>
+      <c r="Q20" s="15"/>
+      <c r="R20" s="15"/>
+      <c r="S20" s="15"/>
       <c r="T20" s="8"/>
       <c r="U20" s="8"/>
       <c r="V20" s="8"/>
@@ -1507,37 +1516,37 @@
         <v>111</v>
       </c>
       <c r="B21" s="8"/>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="E21" s="8" t="s">
+      <c r="E21" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="F21" s="8" t="s">
+      <c r="F21" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="G21" s="8"/>
-      <c r="H21" s="10" t="s">
+      <c r="G21" s="15"/>
+      <c r="H21" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="I21" s="8" t="s">
+      <c r="I21" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="J21" s="8"/>
-      <c r="K21" s="12" t="s">
+      <c r="J21" s="15"/>
+      <c r="K21" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="L21" s="12"/>
-      <c r="M21" s="12"/>
-      <c r="N21" s="8"/>
-      <c r="O21" s="8"/>
-      <c r="P21" s="8"/>
-      <c r="Q21" s="8"/>
-      <c r="R21" s="8"/>
-      <c r="S21" s="8"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="13"/>
+      <c r="N21" s="15"/>
+      <c r="O21" s="15"/>
+      <c r="P21" s="15"/>
+      <c r="Q21" s="15"/>
+      <c r="R21" s="15"/>
+      <c r="S21" s="15"/>
       <c r="T21" s="8"/>
       <c r="U21" s="8"/>
       <c r="V21" s="8"/>
@@ -1552,37 +1561,37 @@
         <v>111</v>
       </c>
       <c r="B22" s="8"/>
-      <c r="C22" s="8" t="s">
+      <c r="C22" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="E22" s="8" t="s">
+      <c r="E22" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="F22" s="8" t="s">
+      <c r="F22" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="G22" s="8"/>
-      <c r="H22" s="10" t="s">
+      <c r="G22" s="15"/>
+      <c r="H22" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="I22" s="8" t="s">
+      <c r="I22" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="J22" s="8"/>
-      <c r="K22" s="12" t="s">
+      <c r="J22" s="15"/>
+      <c r="K22" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="L22" s="12"/>
-      <c r="M22" s="12"/>
-      <c r="N22" s="8"/>
-      <c r="O22" s="8"/>
-      <c r="P22" s="8"/>
-      <c r="Q22" s="8"/>
-      <c r="R22" s="8"/>
-      <c r="S22" s="8"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="13"/>
+      <c r="N22" s="15"/>
+      <c r="O22" s="15"/>
+      <c r="P22" s="15"/>
+      <c r="Q22" s="15"/>
+      <c r="R22" s="15"/>
+      <c r="S22" s="15"/>
       <c r="T22" s="8"/>
       <c r="U22" s="8"/>
       <c r="V22" s="8"/>
@@ -1597,27 +1606,27 @@
         <v>110</v>
       </c>
       <c r="B23" s="8"/>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="D23" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
-      <c r="J23" s="8"/>
-      <c r="K23" s="8"/>
-      <c r="L23" s="8"/>
-      <c r="M23" s="8"/>
-      <c r="N23" s="8"/>
-      <c r="O23" s="8"/>
-      <c r="P23" s="8"/>
-      <c r="Q23" s="8"/>
-      <c r="R23" s="8"/>
-      <c r="S23" s="8"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="15"/>
+      <c r="L23" s="15"/>
+      <c r="M23" s="15"/>
+      <c r="N23" s="15"/>
+      <c r="O23" s="15"/>
+      <c r="P23" s="15"/>
+      <c r="Q23" s="15"/>
+      <c r="R23" s="15"/>
+      <c r="S23" s="15"/>
       <c r="T23" s="8"/>
       <c r="U23" s="8"/>
       <c r="V23" s="8"/>
@@ -1632,27 +1641,27 @@
         <v>110</v>
       </c>
       <c r="B24" s="8"/>
-      <c r="C24" s="8" t="s">
+      <c r="C24" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8"/>
-      <c r="K24" s="8"/>
-      <c r="L24" s="8"/>
-      <c r="M24" s="8"/>
-      <c r="N24" s="8"/>
-      <c r="O24" s="8"/>
-      <c r="P24" s="8"/>
-      <c r="Q24" s="8"/>
-      <c r="R24" s="8"/>
-      <c r="S24" s="8"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="15"/>
+      <c r="K24" s="15"/>
+      <c r="L24" s="15"/>
+      <c r="M24" s="15"/>
+      <c r="N24" s="15"/>
+      <c r="O24" s="15"/>
+      <c r="P24" s="15"/>
+      <c r="Q24" s="15"/>
+      <c r="R24" s="15"/>
+      <c r="S24" s="15"/>
       <c r="T24" s="8"/>
       <c r="U24" s="8"/>
       <c r="V24" s="8"/>
@@ -1667,27 +1676,27 @@
         <v>110</v>
       </c>
       <c r="B25" s="8"/>
-      <c r="C25" s="8" t="s">
+      <c r="C25" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="D25" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
-      <c r="K25" s="8"/>
-      <c r="L25" s="8"/>
-      <c r="M25" s="8"/>
-      <c r="N25" s="8"/>
-      <c r="O25" s="8"/>
-      <c r="P25" s="8"/>
-      <c r="Q25" s="8"/>
-      <c r="R25" s="8"/>
-      <c r="S25" s="8"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15"/>
+      <c r="I25" s="15"/>
+      <c r="J25" s="15"/>
+      <c r="K25" s="15"/>
+      <c r="L25" s="15"/>
+      <c r="M25" s="15"/>
+      <c r="N25" s="15"/>
+      <c r="O25" s="15"/>
+      <c r="P25" s="15"/>
+      <c r="Q25" s="15"/>
+      <c r="R25" s="15"/>
+      <c r="S25" s="15"/>
       <c r="T25" s="8"/>
       <c r="U25" s="8"/>
       <c r="V25" s="8"/>
@@ -1702,27 +1711,27 @@
         <v>110</v>
       </c>
       <c r="B26" s="8"/>
-      <c r="C26" s="8" t="s">
+      <c r="C26" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="D26" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8"/>
-      <c r="K26" s="8"/>
-      <c r="L26" s="8"/>
-      <c r="M26" s="8"/>
-      <c r="N26" s="8"/>
-      <c r="O26" s="8"/>
-      <c r="P26" s="8"/>
-      <c r="Q26" s="8"/>
-      <c r="R26" s="8"/>
-      <c r="S26" s="8"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="15"/>
+      <c r="I26" s="15"/>
+      <c r="J26" s="15"/>
+      <c r="K26" s="15"/>
+      <c r="L26" s="15"/>
+      <c r="M26" s="15"/>
+      <c r="N26" s="15"/>
+      <c r="O26" s="15"/>
+      <c r="P26" s="15"/>
+      <c r="Q26" s="15"/>
+      <c r="R26" s="15"/>
+      <c r="S26" s="15"/>
       <c r="T26" s="8"/>
       <c r="U26" s="8"/>
       <c r="V26" s="8"/>
@@ -1737,27 +1746,27 @@
         <v>110</v>
       </c>
       <c r="B27" s="8"/>
-      <c r="C27" s="8" t="s">
+      <c r="C27" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="D27" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="8"/>
-      <c r="J27" s="8"/>
-      <c r="K27" s="8"/>
-      <c r="L27" s="8"/>
-      <c r="M27" s="8"/>
-      <c r="N27" s="8"/>
-      <c r="O27" s="8"/>
-      <c r="P27" s="8"/>
-      <c r="Q27" s="8"/>
-      <c r="R27" s="8"/>
-      <c r="S27" s="8"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="15"/>
+      <c r="J27" s="15"/>
+      <c r="K27" s="15"/>
+      <c r="L27" s="15"/>
+      <c r="M27" s="15"/>
+      <c r="N27" s="15"/>
+      <c r="O27" s="15"/>
+      <c r="P27" s="15"/>
+      <c r="Q27" s="15"/>
+      <c r="R27" s="15"/>
+      <c r="S27" s="15"/>
       <c r="T27" s="8"/>
       <c r="U27" s="8"/>
       <c r="V27" s="8"/>
@@ -1772,27 +1781,27 @@
         <v>110</v>
       </c>
       <c r="B28" s="8"/>
-      <c r="C28" s="8" t="s">
+      <c r="C28" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="D28" s="8" t="s">
+      <c r="D28" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
-      <c r="K28" s="8"/>
-      <c r="L28" s="8"/>
-      <c r="M28" s="8"/>
-      <c r="N28" s="8"/>
-      <c r="O28" s="8"/>
-      <c r="P28" s="8"/>
-      <c r="Q28" s="8"/>
-      <c r="R28" s="8"/>
-      <c r="S28" s="8"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="15"/>
+      <c r="J28" s="15"/>
+      <c r="K28" s="15"/>
+      <c r="L28" s="15"/>
+      <c r="M28" s="15"/>
+      <c r="N28" s="15"/>
+      <c r="O28" s="15"/>
+      <c r="P28" s="15"/>
+      <c r="Q28" s="15"/>
+      <c r="R28" s="15"/>
+      <c r="S28" s="15"/>
       <c r="T28" s="8"/>
       <c r="U28" s="8"/>
       <c r="V28" s="8"/>
@@ -1807,27 +1816,27 @@
         <v>104</v>
       </c>
       <c r="B29" s="8"/>
-      <c r="C29" s="8" t="s">
+      <c r="C29" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="D29" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
-      <c r="K29" s="8"/>
-      <c r="L29" s="8"/>
-      <c r="M29" s="8"/>
-      <c r="N29" s="8"/>
-      <c r="O29" s="8"/>
-      <c r="P29" s="8"/>
-      <c r="Q29" s="8"/>
-      <c r="R29" s="8"/>
-      <c r="S29" s="8"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="15"/>
+      <c r="I29" s="15"/>
+      <c r="J29" s="15"/>
+      <c r="K29" s="15"/>
+      <c r="L29" s="15"/>
+      <c r="M29" s="15"/>
+      <c r="N29" s="15"/>
+      <c r="O29" s="15"/>
+      <c r="P29" s="15"/>
+      <c r="Q29" s="15"/>
+      <c r="R29" s="15"/>
+      <c r="S29" s="15"/>
       <c r="T29" s="8"/>
       <c r="U29" s="8"/>
       <c r="V29" s="8"/>
@@ -1842,27 +1851,27 @@
         <v>104</v>
       </c>
       <c r="B30" s="8"/>
-      <c r="C30" s="8" t="s">
+      <c r="C30" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="D30" s="8" t="s">
+      <c r="D30" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="8"/>
-      <c r="K30" s="8"/>
-      <c r="L30" s="8"/>
-      <c r="M30" s="8"/>
-      <c r="N30" s="8"/>
-      <c r="O30" s="8"/>
-      <c r="P30" s="8"/>
-      <c r="Q30" s="8"/>
-      <c r="R30" s="8"/>
-      <c r="S30" s="8"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="15"/>
+      <c r="I30" s="15"/>
+      <c r="J30" s="15"/>
+      <c r="K30" s="15"/>
+      <c r="L30" s="15"/>
+      <c r="M30" s="15"/>
+      <c r="N30" s="15"/>
+      <c r="O30" s="15"/>
+      <c r="P30" s="15"/>
+      <c r="Q30" s="15"/>
+      <c r="R30" s="15"/>
+      <c r="S30" s="15"/>
       <c r="T30" s="8"/>
       <c r="U30" s="8"/>
       <c r="V30" s="8"/>
@@ -1877,27 +1886,27 @@
         <v>104</v>
       </c>
       <c r="B31" s="8"/>
-      <c r="C31" s="8" t="s">
+      <c r="C31" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="D31" s="8" t="s">
+      <c r="D31" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
-      <c r="K31" s="8"/>
-      <c r="L31" s="8"/>
-      <c r="M31" s="8"/>
-      <c r="N31" s="8"/>
-      <c r="O31" s="8"/>
-      <c r="P31" s="8"/>
-      <c r="Q31" s="8"/>
-      <c r="R31" s="8"/>
-      <c r="S31" s="8"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="15"/>
+      <c r="I31" s="15"/>
+      <c r="J31" s="15"/>
+      <c r="K31" s="15"/>
+      <c r="L31" s="15"/>
+      <c r="M31" s="15"/>
+      <c r="N31" s="15"/>
+      <c r="O31" s="15"/>
+      <c r="P31" s="15"/>
+      <c r="Q31" s="15"/>
+      <c r="R31" s="15"/>
+      <c r="S31" s="15"/>
       <c r="T31" s="8"/>
       <c r="U31" s="8"/>
       <c r="V31" s="8"/>
@@ -1910,23 +1919,23 @@
     <row r="32" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A32" s="10"/>
       <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="8"/>
-      <c r="I32" s="8"/>
-      <c r="J32" s="8"/>
-      <c r="K32" s="8"/>
-      <c r="L32" s="8"/>
-      <c r="M32" s="8"/>
-      <c r="N32" s="8"/>
-      <c r="O32" s="8"/>
-      <c r="P32" s="8"/>
-      <c r="Q32" s="8"/>
-      <c r="R32" s="8"/>
-      <c r="S32" s="8"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="15"/>
+      <c r="J32" s="15"/>
+      <c r="K32" s="15"/>
+      <c r="L32" s="15"/>
+      <c r="M32" s="15"/>
+      <c r="N32" s="15"/>
+      <c r="O32" s="15"/>
+      <c r="P32" s="15"/>
+      <c r="Q32" s="15"/>
+      <c r="R32" s="15"/>
+      <c r="S32" s="15"/>
       <c r="T32" s="8"/>
       <c r="U32" s="8"/>
       <c r="V32" s="8"/>
@@ -1950,18 +1959,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="K21:M21"/>
-    <mergeCell ref="K22:M22"/>
-    <mergeCell ref="K16:M16"/>
-    <mergeCell ref="K17:M17"/>
-    <mergeCell ref="K18:M18"/>
-    <mergeCell ref="K19:M19"/>
-    <mergeCell ref="K20:M20"/>
-    <mergeCell ref="K11:M11"/>
-    <mergeCell ref="K12:M12"/>
-    <mergeCell ref="K13:M13"/>
-    <mergeCell ref="K14:M14"/>
-    <mergeCell ref="K15:M15"/>
     <mergeCell ref="F16:G16"/>
     <mergeCell ref="I11:J11"/>
     <mergeCell ref="I12:J12"/>
@@ -1974,6 +1971,18 @@
     <mergeCell ref="F13:G13"/>
     <mergeCell ref="F14:G14"/>
     <mergeCell ref="F15:G15"/>
+    <mergeCell ref="K11:M11"/>
+    <mergeCell ref="K12:M12"/>
+    <mergeCell ref="K13:M13"/>
+    <mergeCell ref="K14:M14"/>
+    <mergeCell ref="K15:M15"/>
+    <mergeCell ref="K21:M21"/>
+    <mergeCell ref="K22:M22"/>
+    <mergeCell ref="K16:M16"/>
+    <mergeCell ref="K17:M17"/>
+    <mergeCell ref="K18:M18"/>
+    <mergeCell ref="K19:M19"/>
+    <mergeCell ref="K20:M20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>